<commit_message>
CAD changes and electrical updates
</commit_message>
<xml_diff>
--- a/BoM/BOM_automated_MEW_platform.xlsx
+++ b/BoM/BOM_automated_MEW_platform.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://connectqutedu-my.sharepoint.com/personal/n8448779_qut_edu_au/Documents/My papers/Hardware X - MEW platform/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github repo\automated_mew_platform\BoM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="845" documentId="8_{18974021-8CC7-4730-AE8D-7ACC343B4F49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F2E77873-7927-4623-ACA9-B279ADF99728}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D57FC5A-2FC1-491E-BBAE-EBFE9B5DEE52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="2010" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{B4054C14-A606-4C73-B9F1-21780D16DF14}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B4054C14-A606-4C73-B9F1-21780D16DF14}"/>
   </bookViews>
   <sheets>
     <sheet name="Mechanical" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="363">
   <si>
     <t>Component</t>
   </si>
@@ -280,9 +280,6 @@
     <t>1/4" x 8mm Flexible Coupling</t>
   </si>
   <si>
-    <t>http://openbuildspartstore.com/1-4-x-8mm-flexible-coupling/</t>
-  </si>
-  <si>
     <t>SKU 155</t>
   </si>
   <si>
@@ -632,9 +629,6 @@
   </si>
   <si>
     <t>Profile 20 x 20 mm (slot 6 mm)</t>
-  </si>
-  <si>
-    <t>Profile 20 x 80 mm (V slot)</t>
   </si>
   <si>
     <r>
@@ -1447,12 +1441,76 @@
   <si>
     <t>68W 5VDC &amp; 24VDC dual output switching power supply (RD-65B)</t>
   </si>
+  <si>
+    <t>Profile 20 x80 mm (V slot)</t>
+  </si>
+  <si>
+    <t>Nut M5</t>
+  </si>
+  <si>
+    <t>Low profile M5x15</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SCREWS-M5-LP-15/10 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pack of 10</t>
+    </r>
+  </si>
+  <si>
+    <t>Teflon</t>
+  </si>
+  <si>
+    <t>Brass ring</t>
+  </si>
+  <si>
+    <t>Enclosure</t>
+  </si>
+  <si>
+    <t>USB to TTL Serial Cable</t>
+  </si>
+  <si>
+    <t>ADA954</t>
+  </si>
+  <si>
+    <t>329-7178</t>
+  </si>
+  <si>
+    <t>111-3066</t>
+  </si>
+  <si>
+    <t>DIN rail Omron 5 Pin Relay Socket</t>
+  </si>
+  <si>
+    <t>Omron 24VDC coil non-latching relay SPDT, 10A</t>
+  </si>
+  <si>
+    <t>Black Shorting Link for DIN rail terminals</t>
+  </si>
+  <si>
+    <t>Red Shorting Link for DIN rail terminals</t>
+  </si>
+  <si>
+    <t>P2469</t>
+  </si>
+  <si>
+    <t>P2463</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1492,6 +1550,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1519,7 +1585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1530,6 +1596,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1555,8 +1622,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E1D3A3FC-076F-4DBE-A2CA-BCF9C1B818FB}" name="Table2" displayName="Table2" ref="A1:F99" totalsRowShown="0">
-  <autoFilter ref="A1:F99" xr:uid="{C8CA85C9-3463-4836-A3EB-57FFC2AB0244}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E1D3A3FC-076F-4DBE-A2CA-BCF9C1B818FB}" name="Table2" displayName="Table2" ref="A1:F98" totalsRowShown="0">
+  <autoFilter ref="A1:F98" xr:uid="{C8CA85C9-3463-4836-A3EB-57FFC2AB0244}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{80395295-FF2A-47AE-AF0D-06B3C609ADD6}" name="Componenet"/>
     <tableColumn id="2" xr3:uid="{99C7BD2A-DD73-48A9-AFBD-D3A4E4EFBBA7}" name="Source"/>
@@ -1572,8 +1639,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2EE5CDA5-8D0B-4B71-9252-D3094A7035A5}" name="Table3" displayName="Table3" ref="A1:F82" totalsRowShown="0">
-  <autoFilter ref="A1:F82" xr:uid="{177A9E44-F6DC-4EF6-9651-CDAA645EE035}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2EE5CDA5-8D0B-4B71-9252-D3094A7035A5}" name="Table3" displayName="Table3" ref="A1:F75" totalsRowShown="0">
+  <autoFilter ref="A1:F75" xr:uid="{177A9E44-F6DC-4EF6-9651-CDAA645EE035}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{68B58E8D-CFF5-46C4-9AB7-7EDB0A1BD3D5}" name="Component"/>
     <tableColumn id="2" xr3:uid="{D5B59500-3BE1-4C27-8039-126CCDFEAC2B}" name="Source"/>
@@ -1885,10 +1952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{502BC3CC-4DC8-4EA2-ADB9-DF1E4F84FB7E}">
-  <dimension ref="A1:M101"/>
+  <dimension ref="A1:M100"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,13 +2021,13 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D3">
         <v>19.463999999999999</v>
@@ -1987,13 +2054,13 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D4">
         <v>2.21</v>
@@ -2020,23 +2087,23 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>346</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>22.97</v>
+        <v>22.82</v>
       </c>
       <c r="F5" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
-        <v>22.97</v>
+        <v>45.64</v>
       </c>
       <c r="J5">
         <v>6</v>
@@ -2062,14 +2129,14 @@
         <v>11</v>
       </c>
       <c r="D6">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E6">
         <v>2.16</v>
       </c>
       <c r="F6" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
-        <v>95.04</v>
+        <v>108</v>
       </c>
       <c r="J6">
         <v>6</v>
@@ -2095,14 +2162,14 @@
         <v>12</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="E7">
         <v>1.66</v>
       </c>
       <c r="F7" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
-        <v>9.9599999999999991</v>
+        <v>66.399999999999991</v>
       </c>
       <c r="J7">
         <v>8</v>
@@ -2118,21 +2185,24 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>191</v>
+      <c r="A8" s="4" t="s">
+        <v>190</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>202</v>
+        <v>200</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
       </c>
       <c r="E8">
         <v>3.08</v>
       </c>
       <c r="F8" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
-        <v>0</v>
+        <v>61.6</v>
       </c>
       <c r="J8">
         <v>3</v>
@@ -2148,21 +2218,24 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>192</v>
+      <c r="A9" s="4" t="s">
+        <v>191</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
       </c>
       <c r="E9">
         <v>3.08</v>
       </c>
       <c r="F9" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
-        <v>0</v>
+        <v>61.6</v>
       </c>
       <c r="J9">
         <v>6</v>
@@ -2179,317 +2252,335 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>195</v>
+        <v>347</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>204</v>
+        <v>202</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
       </c>
       <c r="E10">
         <v>3.85</v>
       </c>
       <c r="F10" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>6</v>
-      </c>
-      <c r="K10" t="s">
-        <v>52</v>
-      </c>
-      <c r="L10" t="s">
-        <v>53</v>
-      </c>
-      <c r="M10" t="s">
-        <v>54</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>194</v>
       </c>
       <c r="B11" t="s">
-        <v>337</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>202</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11">
-        <v>9.84</v>
+        <v>3.85</v>
       </c>
       <c r="F11" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
-        <v>9.84</v>
+        <v>7.7</v>
       </c>
       <c r="J11">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>193</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>335</v>
       </c>
       <c r="C12" t="s">
-        <v>205</v>
+        <v>16</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>4.62</v>
+        <v>9.84</v>
       </c>
       <c r="F12" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
-        <v>0</v>
+        <v>9.84</v>
       </c>
       <c r="J12">
         <v>10</v>
       </c>
       <c r="K12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="M12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>206</v>
+        <v>203</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
       </c>
       <c r="E13">
-        <v>2.89</v>
+        <v>4.62</v>
       </c>
       <c r="F13" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
-        <v>0</v>
+        <v>9.24</v>
       </c>
       <c r="J13">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="M13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>193</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>204</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E14">
-        <v>3.39</v>
+        <v>2.89</v>
       </c>
       <c r="F14" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
-        <v>10.17</v>
+        <v>5.78</v>
       </c>
       <c r="J14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="M14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>348</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>349</v>
       </c>
       <c r="D15">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E15">
-        <v>11.93</v>
+        <v>1.38</v>
       </c>
       <c r="F15" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
-        <v>71.58</v>
-      </c>
-      <c r="J15">
-        <v>6</v>
-      </c>
-      <c r="K15" t="s">
-        <v>67</v>
-      </c>
-      <c r="L15" t="s">
-        <v>68</v>
-      </c>
-      <c r="M15" t="s">
-        <v>69</v>
+        <v>13.799999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>21</v>
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>3.39</v>
       </c>
       <c r="F16" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
-        <v>0</v>
+        <v>10.17</v>
       </c>
       <c r="J16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="L16" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="M16" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>326</v>
+      <c r="A17" t="s">
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>328</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>303</v>
+        <v>20</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E17">
-        <v>15.26</v>
+        <v>11.93</v>
       </c>
       <c r="F17" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
-        <v>15.26</v>
+        <v>71.58</v>
+      </c>
+      <c r="J17">
+        <v>6</v>
+      </c>
+      <c r="K17" t="s">
+        <v>67</v>
+      </c>
+      <c r="L17" t="s">
+        <v>68</v>
+      </c>
+      <c r="M17" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="B18" t="s">
-        <v>323</v>
-      </c>
-      <c r="C18" t="s">
-        <v>324</v>
-      </c>
-      <c r="D18">
-        <v>3</v>
-      </c>
-      <c r="E18">
-        <v>125.38</v>
+      <c r="A18" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F18" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
-        <v>376.14</v>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
+      <c r="K18" t="s">
+        <v>70</v>
+      </c>
+      <c r="L18" t="s">
+        <v>71</v>
+      </c>
+      <c r="M18" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B19" t="s">
+        <v>326</v>
+      </c>
+      <c r="C19" t="s">
+        <v>301</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>15.26</v>
+      </c>
       <c r="F19" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
+        <v>15.26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="A20" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="F20" s="1">
+        <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
         <v>0</v>
       </c>
-      <c r="J19">
-        <v>4</v>
-      </c>
-      <c r="K19" t="s">
-        <v>73</v>
-      </c>
-      <c r="L19" t="s">
-        <v>74</v>
-      </c>
-      <c r="M19" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A20" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="J20">
-        <v>8</v>
-      </c>
-      <c r="K20" t="s">
-        <v>76</v>
-      </c>
-      <c r="L20" t="s">
-        <v>77</v>
-      </c>
-      <c r="M20" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="B21" t="s">
+        <v>321</v>
+      </c>
+      <c r="C21" t="s">
+        <v>322</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>125.38</v>
+      </c>
       <c r="F21" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>3</v>
-      </c>
-      <c r="K21" t="s">
-        <v>79</v>
-      </c>
-      <c r="L21" t="s">
-        <v>80</v>
-      </c>
-      <c r="M21" t="s">
-        <v>81</v>
+        <v>376.14</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
       <c r="F22" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
       <c r="F23" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
         <v>0</v>
@@ -2500,1144 +2591,1183 @@
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F25" s="1">
-        <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
-        <v>0</v>
+      <c r="J24">
+        <v>4</v>
+      </c>
+      <c r="K24" t="s">
+        <v>73</v>
+      </c>
+      <c r="L24" t="s">
+        <v>74</v>
+      </c>
+      <c r="M24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A25" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="J25">
+        <v>8</v>
+      </c>
+      <c r="K25" t="s">
+        <v>76</v>
+      </c>
+      <c r="L25" t="s">
+        <v>77</v>
+      </c>
+      <c r="M25" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>350</v>
+      </c>
       <c r="F26" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>351</v>
+      </c>
       <c r="F27" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F28" s="1">
+    <row r="28" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="J28">
+        <v>2</v>
+      </c>
+      <c r="K28" t="s">
+        <v>81</v>
+      </c>
+      <c r="L28" t="s">
+        <v>82</v>
+      </c>
+      <c r="M28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>549.99</v>
+      </c>
+      <c r="F29" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F29" s="1"/>
+        <v>549.99</v>
+      </c>
       <c r="J29">
         <v>2</v>
       </c>
       <c r="K29" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L29" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M29" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="A30" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" t="s">
         <v>13</v>
       </c>
-      <c r="C30" t="s">
-        <v>25</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <v>549.99</v>
-      </c>
-      <c r="F30" s="1">
-        <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
-        <v>549.99</v>
-      </c>
-      <c r="J30">
-        <v>2</v>
-      </c>
-      <c r="K30" t="s">
-        <v>85</v>
-      </c>
-      <c r="L30" t="s">
-        <v>86</v>
-      </c>
-      <c r="M30" t="s">
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31">
+        <v>8</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="F31" s="1"/>
+      <c r="L31" t="s">
+        <v>88</v>
+      </c>
+      <c r="M31" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>26</v>
+      <c r="A32" t="s">
+        <v>28</v>
       </c>
       <c r="B32" t="s">
         <v>13</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D32">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F32" s="1"/>
       <c r="J32">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K32" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="L32" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="M32" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
         <v>13</v>
       </c>
       <c r="C33" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D33">
         <v>6</v>
       </c>
       <c r="F33" s="1"/>
       <c r="J33">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K33" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L33" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="M33" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B34" t="s">
         <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D34">
         <v>6</v>
       </c>
       <c r="F34" s="1"/>
       <c r="J34">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="K34" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L34" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="M34" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
         <v>13</v>
       </c>
       <c r="C35" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D35">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F35" s="1"/>
       <c r="J35">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="K35" t="s">
+        <v>99</v>
+      </c>
+      <c r="L35" t="s">
         <v>97</v>
       </c>
-      <c r="L35" t="s">
-        <v>98</v>
-      </c>
       <c r="M35" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B36" t="s">
         <v>13</v>
       </c>
       <c r="C36" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D36">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F36" s="1"/>
       <c r="J36">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="K36" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M36" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B37" t="s">
         <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D37">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F37" s="1"/>
       <c r="J37">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="K37" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M37" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B38" t="s">
         <v>13</v>
       </c>
       <c r="C38" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D38">
         <v>6</v>
       </c>
       <c r="F38" s="1"/>
       <c r="J38">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K38" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M38" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>189</v>
       </c>
       <c r="B39" t="s">
         <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>54</v>
+        <v>205</v>
       </c>
       <c r="D39">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F39" s="1"/>
       <c r="J39">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="K39" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="L39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M39" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>190</v>
+        <v>58</v>
       </c>
       <c r="B40" t="s">
         <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>207</v>
+        <v>60</v>
       </c>
       <c r="D40">
         <v>10</v>
       </c>
       <c r="F40" s="1"/>
       <c r="J40">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="K40" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L40" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="M40" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B41" t="s">
         <v>13</v>
       </c>
       <c r="C41" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D41">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F41" s="1"/>
       <c r="J41">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K41" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="L41" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M41" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B42" t="s">
         <v>13</v>
       </c>
       <c r="C42" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D42">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F42" s="1"/>
       <c r="J42">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K42" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L42" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="M42" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B43" t="s">
         <v>13</v>
       </c>
       <c r="C43" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F43" s="1"/>
       <c r="J43">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K43" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="L43" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="M43" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B44" t="s">
         <v>13</v>
       </c>
       <c r="C44" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D44">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F44" s="1"/>
       <c r="J44">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="K44" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="L44" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="M44" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B45" t="s">
         <v>13</v>
       </c>
       <c r="C45" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D45">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F45" s="1"/>
       <c r="J45">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="K45" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="L45" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="M45" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B46" t="s">
         <v>13</v>
       </c>
       <c r="C46" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D46">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F46" s="1"/>
       <c r="J46">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K46" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="L46" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="M46" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B47" t="s">
         <v>13</v>
       </c>
       <c r="C47" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D47">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F47" s="1"/>
       <c r="J47">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K47" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="L47" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="M47" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B48" t="s">
         <v>13</v>
       </c>
       <c r="C48" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D48">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" s="1"/>
       <c r="J48">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="K48" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="L48" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="M48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B49" t="s">
         <v>13</v>
       </c>
       <c r="C49" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D49">
         <v>2</v>
       </c>
       <c r="F49" s="1"/>
       <c r="J49">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K49" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L49" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="M49" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B50" t="s">
         <v>13</v>
       </c>
       <c r="C50" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" s="1"/>
       <c r="J50">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K50" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="L50" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="M50" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B51" t="s">
         <v>13</v>
       </c>
       <c r="C51" t="s">
-        <v>90</v>
+        <v>218</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F51" s="1"/>
       <c r="J51">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K51" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="L51" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="M51" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B52" t="s">
         <v>13</v>
       </c>
       <c r="C52" t="s">
-        <v>220</v>
+        <v>95</v>
       </c>
       <c r="D52">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F52" s="1"/>
       <c r="J52">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K52" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="L52" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="M52" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B53" t="s">
         <v>13</v>
       </c>
       <c r="C53" t="s">
-        <v>96</v>
+        <v>206</v>
       </c>
       <c r="D53">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="F53" s="1"/>
       <c r="J53">
         <v>1</v>
       </c>
       <c r="K53" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="L53" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="M53" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B54" t="s">
         <v>13</v>
       </c>
       <c r="C54" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D54">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="F54" s="1"/>
       <c r="J54">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K54" t="s">
+        <v>151</v>
+      </c>
+      <c r="L54" t="s">
         <v>149</v>
       </c>
-      <c r="L54" t="s">
-        <v>150</v>
-      </c>
       <c r="M54" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B55" t="s">
         <v>13</v>
       </c>
       <c r="C55" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D55">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="F55" s="1"/>
       <c r="J55">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K55" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="L55" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="M55" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B56" t="s">
         <v>13</v>
       </c>
       <c r="C56" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D56">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="F56" s="1"/>
       <c r="J56">
         <v>1</v>
       </c>
       <c r="K56" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="L56" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="M56" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B57" t="s">
         <v>13</v>
       </c>
       <c r="C57" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D57">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F57" s="1"/>
       <c r="J57">
         <v>1</v>
       </c>
       <c r="K57" t="s">
+        <v>159</v>
+      </c>
+      <c r="L57" t="s">
         <v>157</v>
       </c>
-      <c r="L57" t="s">
+      <c r="M57" t="s">
         <v>158</v>
-      </c>
-      <c r="M57" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B58" t="s">
         <v>13</v>
       </c>
       <c r="C58" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D58">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="F58" s="1"/>
       <c r="J58">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K58" t="s">
         <v>160</v>
       </c>
       <c r="L58" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="M58" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B59" t="s">
         <v>13</v>
       </c>
       <c r="C59" t="s">
-        <v>213</v>
+        <v>111</v>
       </c>
       <c r="D59">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F59" s="1"/>
       <c r="J59">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K59" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="L59" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="M59" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B60" t="s">
         <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D60">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F60" s="1"/>
       <c r="J60">
         <v>3</v>
       </c>
       <c r="K60" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="L60" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="M60" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B61" t="s">
         <v>13</v>
       </c>
       <c r="C61" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D61">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F61" s="1"/>
       <c r="J61">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K61" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="L61" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="M61" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B62" t="s">
         <v>13</v>
       </c>
       <c r="C62" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" s="1"/>
       <c r="J62">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K62" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="L62" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="M62" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B63" t="s">
         <v>13</v>
       </c>
       <c r="C63" t="s">
-        <v>121</v>
+        <v>212</v>
       </c>
       <c r="D63">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="F63" s="1"/>
       <c r="J63">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K63" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="L63" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="M63" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B64" t="s">
         <v>13</v>
       </c>
       <c r="C64" t="s">
-        <v>214</v>
+        <v>126</v>
       </c>
       <c r="D64">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="F64" s="1"/>
       <c r="J64">
         <v>1</v>
       </c>
       <c r="K64" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="L64" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="M64" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B65" t="s">
         <v>13</v>
       </c>
       <c r="C65" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D65">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F65" s="1"/>
       <c r="J65">
         <v>1</v>
       </c>
       <c r="K65" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="L65" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="M65" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B66" t="s">
         <v>13</v>
       </c>
       <c r="C66" t="s">
-        <v>130</v>
+        <v>213</v>
       </c>
       <c r="D66">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F66" s="1"/>
       <c r="J66">
         <v>1</v>
       </c>
       <c r="K66" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="L66" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="M66" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B67" t="s">
         <v>13</v>
       </c>
       <c r="C67" t="s">
-        <v>215</v>
+        <v>135</v>
       </c>
       <c r="D67">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F67" s="1"/>
       <c r="J67">
         <v>1</v>
       </c>
       <c r="K67" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="L67" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="M67" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B68" t="s">
         <v>13</v>
       </c>
       <c r="C68" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F68" s="1"/>
       <c r="J68">
-        <v>1</v>
-      </c>
-      <c r="K68" t="s">
-        <v>187</v>
-      </c>
-      <c r="L68" t="s">
-        <v>188</v>
-      </c>
-      <c r="M68" t="s">
-        <v>189</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B69" t="s">
         <v>13</v>
       </c>
       <c r="C69" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D69">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F69" s="1"/>
-      <c r="J69">
-        <v>0</v>
-      </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B70" t="s">
         <v>13</v>
       </c>
       <c r="C70" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F70" s="1"/>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B71" t="s">
         <v>13</v>
       </c>
       <c r="C71" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D71">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F71" s="1"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B72" t="s">
         <v>13</v>
       </c>
       <c r="C72" t="s">
-        <v>148</v>
+        <v>214</v>
       </c>
       <c r="D72">
         <v>1</v>
@@ -3646,43 +3776,43 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B73" t="s">
         <v>13</v>
       </c>
       <c r="C73" t="s">
-        <v>216</v>
+        <v>152</v>
       </c>
       <c r="D73">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F73" s="1"/>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B74" t="s">
         <v>13</v>
       </c>
       <c r="C74" t="s">
-        <v>153</v>
+        <v>216</v>
       </c>
       <c r="D74">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F74" s="1"/>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B75" t="s">
         <v>13</v>
       </c>
       <c r="C75" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -3691,13 +3821,13 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B76" t="s">
         <v>13</v>
       </c>
       <c r="C76" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -3712,37 +3842,37 @@
         <v>13</v>
       </c>
       <c r="C77" t="s">
-        <v>217</v>
+        <v>162</v>
       </c>
       <c r="D77">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F77" s="1"/>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B78" t="s">
         <v>13</v>
       </c>
       <c r="C78" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D78">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" s="1"/>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B79" t="s">
         <v>13</v>
       </c>
       <c r="C79" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D79">
         <v>3</v>
@@ -3751,71 +3881,62 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B80" t="s">
         <v>13</v>
       </c>
       <c r="C80" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D80">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" s="1"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>169</v>
-      </c>
-      <c r="B81" t="s">
-        <v>13</v>
-      </c>
-      <c r="C81" t="s">
-        <v>171</v>
-      </c>
-      <c r="D81">
-        <v>2</v>
-      </c>
       <c r="F81" s="1"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A82" s="2" t="s">
+        <v>219</v>
+      </c>
       <c r="F82" s="1"/>
     </row>
-    <row r="83" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A83" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="F83" s="1"/>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>325</v>
+      </c>
+      <c r="B83" t="s">
+        <v>326</v>
+      </c>
+      <c r="C83" t="s">
+        <v>301</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83">
+        <v>7.7</v>
+      </c>
+      <c r="F83" s="1">
+        <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
+        <v>7.7</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>327</v>
+      <c r="A84" s="4" t="s">
+        <v>220</v>
       </c>
       <c r="B84" t="s">
-        <v>328</v>
-      </c>
-      <c r="C84" t="s">
-        <v>303</v>
-      </c>
-      <c r="D84">
-        <v>1</v>
-      </c>
-      <c r="E84">
-        <v>7.7</v>
+        <v>14</v>
       </c>
       <c r="F84" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
-        <v>7.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="B85" t="s">
-        <v>14</v>
-      </c>
       <c r="F85" s="1">
         <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
         <v>0</v>
@@ -3899,16 +4020,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F99" s="1">
-        <f>Table2[[#This Row],[Cost/Unit (USD)]]*Table2[[#This Row],[Quantity]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F101" s="1">
-        <f>SUM(F3:F99)</f>
-        <v>1400.5716599999998</v>
+    <row r="100" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F100" s="1">
+        <f>SUM(F3:F98)</f>
+        <v>1660.0616600000001</v>
       </c>
     </row>
   </sheetData>
@@ -3922,10 +4037,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D242B8A8-C87E-45B6-A870-5B9AB09679FD}">
-  <dimension ref="A1:F82"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3938,7 +4053,7 @@
     <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3958,24 +4073,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F2">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B3" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -3988,15 +4103,15 @@
         <v>188.97</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -4009,30 +4124,45 @@
         <v>40.76</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>353</v>
+      </c>
+      <c r="B5" t="s">
+        <v>330</v>
+      </c>
+      <c r="C5" t="s">
+        <v>354</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>17.18</v>
+      </c>
       <c r="F5">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>34.36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="F6" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
+    <row r="7" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>259</v>
+      </c>
+      <c r="B7" t="s">
         <v>260</v>
       </c>
-      <c r="F6" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>261</v>
-      </c>
-      <c r="B7" t="s">
-        <v>262</v>
-      </c>
       <c r="C7" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -4045,69 +4175,69 @@
         <v>7.41</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="B8" t="s">
+        <v>237</v>
+      </c>
+      <c r="C8" t="s">
         <v>289</v>
       </c>
-      <c r="B8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="F8" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="B9" t="s">
+        <v>237</v>
+      </c>
+      <c r="C9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F9" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="F8" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="B9" t="s">
-        <v>239</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C10" t="s">
         <v>292</v>
       </c>
-      <c r="F9" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="B10" t="s">
-        <v>239</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B11" t="s">
+        <v>237</v>
+      </c>
+      <c r="C11" t="s">
         <v>294</v>
       </c>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>296</v>
+      </c>
+      <c r="B12" t="s">
+        <v>237</v>
+      </c>
+      <c r="C12" t="s">
         <v>295</v>
-      </c>
-      <c r="B11" t="s">
-        <v>239</v>
-      </c>
-      <c r="C11" t="s">
-        <v>296</v>
-      </c>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>298</v>
-      </c>
-      <c r="B12" t="s">
-        <v>239</v>
-      </c>
-      <c r="C12" t="s">
-        <v>297</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -4120,597 +4250,741 @@
         <v>2.68</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>302</v>
+        <v>223</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>300</v>
       </c>
       <c r="B15" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C15" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="F15">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>1148</v>
+      </c>
+      <c r="F15" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>1148</v>
+      </c>
+      <c r="I15">
+        <f>-I23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="6"/>
+    <row r="20" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F21" s="6"/>
+      <c r="A21" t="s">
+        <v>225</v>
+      </c>
+      <c r="B21" t="s">
+        <v>226</v>
+      </c>
+      <c r="C21" t="s">
+        <v>227</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>94.09</v>
+      </c>
+      <c r="F21">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>282.27</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F22" s="6"/>
+      <c r="A22" t="s">
+        <v>253</v>
+      </c>
+      <c r="B22" t="s">
+        <v>226</v>
+      </c>
+      <c r="C22" t="s">
+        <v>254</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>3.03</v>
+      </c>
+      <c r="F22">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>9.09</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>226</v>
+        <v>252</v>
+      </c>
+      <c r="F23" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>227</v>
+        <v>262</v>
       </c>
       <c r="B24" t="s">
-        <v>228</v>
+        <v>263</v>
       </c>
       <c r="C24" t="s">
-        <v>229</v>
+        <v>266</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>94.09</v>
-      </c>
-      <c r="F24">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>282.27</v>
+        <v>1542.95</v>
+      </c>
+      <c r="F24" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>1542.95</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="B25" t="s">
+        <v>263</v>
+      </c>
+      <c r="C25" t="s">
+        <v>265</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1667.21</v>
+      </c>
+      <c r="F25" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>1667.21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>267</v>
+      </c>
+      <c r="B26" t="s">
+        <v>263</v>
+      </c>
+      <c r="C26" t="s">
+        <v>268</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>40</v>
+      </c>
+      <c r="F26" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>269</v>
+      </c>
+      <c r="B27" t="s">
+        <v>263</v>
+      </c>
+      <c r="C27" t="s">
+        <v>270</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>153.16</v>
+      </c>
+      <c r="F27" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>153.16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="C25" t="s">
+      <c r="F28">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="F29">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="F30">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="F31" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="F32">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>248</v>
+      </c>
+      <c r="B33" t="s">
+        <v>333</v>
+      </c>
+      <c r="C33" t="s">
+        <v>249</v>
+      </c>
+      <c r="D33">
+        <v>0.25</v>
+      </c>
+      <c r="E33">
+        <v>39.619999999999997</v>
+      </c>
+      <c r="F33">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>9.9049999999999994</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>246</v>
+      </c>
+      <c r="B34" t="s">
+        <v>330</v>
+      </c>
+      <c r="C34" t="s">
+        <v>247</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>20.81</v>
+      </c>
+      <c r="F34">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>41.62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F35" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>297</v>
+      </c>
+      <c r="B36" t="s">
+        <v>298</v>
+      </c>
+      <c r="C36" t="s">
+        <v>299</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>557</v>
+      </c>
+      <c r="F36" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>557</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="F37" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="F38" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F39" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>256</v>
       </c>
-      <c r="D25">
-        <v>3</v>
-      </c>
-      <c r="E25">
-        <v>3.03</v>
-      </c>
-      <c r="F25">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>9.09</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-    </row>
-    <row r="27" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="F27" s="6">
+      <c r="B40" t="s">
+        <v>334</v>
+      </c>
+      <c r="C40" t="s">
+        <v>257</v>
+      </c>
+      <c r="F40" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>264</v>
-      </c>
-      <c r="B28" t="s">
-        <v>265</v>
-      </c>
-      <c r="C28" t="s">
-        <v>268</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28">
-        <v>1542.95</v>
-      </c>
-      <c r="F28" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>1542.95</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>266</v>
-      </c>
-      <c r="B29" t="s">
-        <v>265</v>
-      </c>
-      <c r="C29" t="s">
-        <v>267</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <v>1667.21</v>
-      </c>
-      <c r="F29" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>1667.21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>269</v>
-      </c>
-      <c r="B30" t="s">
-        <v>265</v>
-      </c>
-      <c r="C30" t="s">
-        <v>270</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <v>40</v>
-      </c>
-      <c r="F30" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>271</v>
-      </c>
-      <c r="B31" t="s">
-        <v>265</v>
-      </c>
-      <c r="C31" t="s">
-        <v>272</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <v>153.16</v>
-      </c>
-      <c r="F31" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>153.16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F32" s="6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F41" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="F33">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F42" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="F34">
+    <row r="43" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F43" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="F35">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="F36">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>250</v>
-      </c>
-      <c r="B37" t="s">
-        <v>335</v>
-      </c>
-      <c r="C37" t="s">
-        <v>251</v>
-      </c>
-      <c r="D37">
-        <v>0.25</v>
-      </c>
-      <c r="E37">
-        <v>39.619999999999997</v>
-      </c>
-      <c r="F37">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>9.9049999999999994</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>248</v>
-      </c>
-      <c r="B38" t="s">
-        <v>332</v>
-      </c>
-      <c r="C38" t="s">
-        <v>249</v>
-      </c>
-      <c r="D38">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>241</v>
+      </c>
+      <c r="B44" t="s">
+        <v>237</v>
+      </c>
+      <c r="C44" t="s">
+        <v>238</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>57.88</v>
+      </c>
+      <c r="F44" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>57.88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>242</v>
+      </c>
+      <c r="B45" t="s">
+        <v>237</v>
+      </c>
+      <c r="C45" t="s">
+        <v>239</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>38.28</v>
+      </c>
+      <c r="F45" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>38.28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>345</v>
+      </c>
+      <c r="B46" t="s">
+        <v>237</v>
+      </c>
+      <c r="C46" t="s">
+        <v>240</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>23.49</v>
+      </c>
+      <c r="F46" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>23.49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>243</v>
+      </c>
+      <c r="B47" t="s">
+        <v>283</v>
+      </c>
+      <c r="C47" t="s">
+        <v>245</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>14.86</v>
+      </c>
+      <c r="F47" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>14.86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>281</v>
+      </c>
+      <c r="B48" t="s">
+        <v>282</v>
+      </c>
+      <c r="C48" t="s">
+        <v>284</v>
+      </c>
+      <c r="D48">
         <v>2</v>
       </c>
-      <c r="E38">
-        <v>20.81</v>
-      </c>
-      <c r="F38">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>41.62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F39" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F40" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F41" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A42" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="F42" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>299</v>
-      </c>
-      <c r="B43" t="s">
-        <v>300</v>
-      </c>
-      <c r="C43" t="s">
-        <v>301</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43">
-        <v>557</v>
-      </c>
-      <c r="F43" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>557</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="F44" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="F45" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F46" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F47" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A48" s="2" t="s">
-        <v>235</v>
+      <c r="E48">
+        <v>2.19</v>
       </c>
       <c r="F48" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
+        <v>4.38</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>258</v>
+        <v>315</v>
       </c>
       <c r="B49" t="s">
-        <v>336</v>
+        <v>244</v>
       </c>
       <c r="C49" t="s">
-        <v>259</v>
+        <v>314</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>7.63</v>
       </c>
       <c r="F49" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
+        <v>7.63</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>236</v>
+      <c r="A50" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="B50" t="s">
+        <v>316</v>
+      </c>
+      <c r="C50" t="s">
+        <v>317</v>
+      </c>
+      <c r="D50">
+        <v>26</v>
+      </c>
+      <c r="E50">
+        <v>2.23</v>
       </c>
       <c r="F50" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
+        <v>57.98</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>280</v>
+      <c r="A51" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="B51" t="s">
+        <v>316</v>
+      </c>
+      <c r="C51" t="s">
+        <v>320</v>
+      </c>
+      <c r="D51">
+        <v>4</v>
+      </c>
+      <c r="E51">
+        <v>4.43</v>
       </c>
       <c r="F51" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
+        <v>17.72</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="B52" t="s">
+        <v>333</v>
+      </c>
+      <c r="C52" t="s">
+        <v>355</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>11.41</v>
+      </c>
       <c r="F52" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A53" s="2" t="s">
-        <v>237</v>
+        <v>11.41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>357</v>
+      </c>
+      <c r="B53" t="s">
+        <v>333</v>
+      </c>
+      <c r="C53" t="s">
+        <v>356</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>7.58</v>
       </c>
       <c r="F53" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
+        <v>7.58</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>243</v>
+        <v>359</v>
       </c>
       <c r="B54" t="s">
-        <v>239</v>
+        <v>316</v>
       </c>
       <c r="C54" t="s">
-        <v>240</v>
+        <v>361</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E54">
-        <v>57.88</v>
+        <v>2.87</v>
       </c>
       <c r="F54" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>57.88</v>
+        <v>5.74</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>244</v>
+        <v>360</v>
       </c>
       <c r="B55" t="s">
-        <v>239</v>
+        <v>316</v>
       </c>
       <c r="C55" t="s">
-        <v>241</v>
+        <v>362</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E55">
-        <v>38.28</v>
+        <v>2.87</v>
       </c>
       <c r="F55" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>38.28</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>347</v>
-      </c>
-      <c r="B56" t="s">
-        <v>239</v>
-      </c>
-      <c r="C56" t="s">
-        <v>242</v>
-      </c>
-      <c r="D56">
-        <v>1</v>
-      </c>
-      <c r="E56">
-        <v>23.49</v>
+        <v>5.74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A56" s="2" t="s">
+        <v>236</v>
       </c>
       <c r="F56" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>23.49</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>245</v>
-      </c>
-      <c r="B57" t="s">
-        <v>285</v>
-      </c>
-      <c r="C57" t="s">
-        <v>247</v>
-      </c>
-      <c r="D57">
-        <v>1</v>
-      </c>
-      <c r="E57">
-        <v>14.86</v>
+      <c r="A57" s="4" t="s">
+        <v>255</v>
       </c>
       <c r="F57" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>14.86</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>283</v>
-      </c>
-      <c r="B58" t="s">
-        <v>284</v>
-      </c>
-      <c r="C58" t="s">
-        <v>286</v>
-      </c>
-      <c r="D58">
-        <v>2</v>
-      </c>
-      <c r="E58">
-        <v>2.19</v>
-      </c>
       <c r="F58" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>4.38</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>317</v>
-      </c>
-      <c r="B59" t="s">
-        <v>246</v>
-      </c>
-      <c r="C59" t="s">
-        <v>316</v>
-      </c>
-      <c r="D59">
-        <v>1</v>
-      </c>
-      <c r="E59">
-        <v>7.63</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A59" s="2" t="s">
+        <v>271</v>
       </c>
       <c r="F59" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>7.63</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>320</v>
+      <c r="A60" t="s">
+        <v>272</v>
       </c>
       <c r="B60" t="s">
-        <v>318</v>
+        <v>330</v>
       </c>
       <c r="C60" t="s">
-        <v>319</v>
+        <v>277</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
       </c>
       <c r="E60">
-        <v>2.23</v>
+        <v>6.63</v>
       </c>
       <c r="F60" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
+        <v>6.63</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>321</v>
+      <c r="A61" t="s">
+        <v>273</v>
       </c>
       <c r="B61" t="s">
-        <v>318</v>
+        <v>330</v>
       </c>
       <c r="C61" t="s">
-        <v>322</v>
+        <v>274</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
       </c>
       <c r="E61">
-        <v>4.43</v>
+        <v>1.38</v>
       </c>
       <c r="F61" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>275</v>
+      </c>
+      <c r="B62" t="s">
+        <v>330</v>
+      </c>
+      <c r="C62" t="s">
+        <v>276</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>1.38</v>
+      </c>
       <c r="F62" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A63" s="2" t="s">
-        <v>238</v>
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>279</v>
       </c>
       <c r="F63" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
@@ -4719,7 +4993,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>257</v>
+        <v>280</v>
       </c>
       <c r="F64" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
@@ -4727,298 +5001,202 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F65" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A66" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="F66" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
+      <c r="A65" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="B65" t="s">
+        <v>340</v>
+      </c>
+      <c r="C65" t="s">
+        <v>342</v>
+      </c>
+      <c r="D65">
+        <v>0.2</v>
+      </c>
+      <c r="E65">
+        <v>78.39</v>
+      </c>
+      <c r="F65" s="1">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>15.678000000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="B66" t="s">
+        <v>340</v>
+      </c>
+      <c r="C66" t="s">
+        <v>341</v>
+      </c>
+      <c r="D66">
+        <v>0.2</v>
+      </c>
+      <c r="E66">
+        <v>50.47</v>
+      </c>
+      <c r="F66" s="1">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>10.094000000000001</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>274</v>
+        <v>302</v>
       </c>
       <c r="B67" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C67" t="s">
-        <v>279</v>
+        <v>308</v>
       </c>
       <c r="D67">
         <v>1</v>
       </c>
       <c r="E67">
-        <v>6.63</v>
+        <v>5.46</v>
       </c>
       <c r="F67" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>6.63</v>
+        <v>5.46</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>275</v>
+        <v>303</v>
       </c>
       <c r="B68" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C68" t="s">
-        <v>276</v>
+        <v>307</v>
       </c>
       <c r="D68">
         <v>1</v>
       </c>
       <c r="E68">
-        <v>1.38</v>
+        <v>13.9</v>
       </c>
       <c r="F68" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>1.38</v>
+        <v>13.9</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>277</v>
+        <v>304</v>
       </c>
       <c r="B69" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C69" t="s">
-        <v>278</v>
+        <v>309</v>
       </c>
       <c r="D69">
         <v>1</v>
       </c>
       <c r="E69">
-        <v>1.38</v>
+        <v>7.62</v>
       </c>
       <c r="F69" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>1.38</v>
+        <v>7.62</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
-        <v>281</v>
+      <c r="A70" t="s">
+        <v>312</v>
+      </c>
+      <c r="B70" t="s">
+        <v>331</v>
+      </c>
+      <c r="C70" t="s">
+        <v>313</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>9.1300000000000008</v>
       </c>
       <c r="F70" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>9.1300000000000008</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>327</v>
+      </c>
+      <c r="B71" t="s">
+        <v>328</v>
+      </c>
+      <c r="C71" t="s">
+        <v>329</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>65.41</v>
+      </c>
+      <c r="F71" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>65.41</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>305</v>
+      </c>
+      <c r="B72" t="s">
+        <v>331</v>
+      </c>
+      <c r="C72" t="s">
+        <v>306</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="F72" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>5.0599999999999996</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>310</v>
+      </c>
+      <c r="B73" t="s">
+        <v>331</v>
+      </c>
+      <c r="C73" t="s">
+        <v>311</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>3.15</v>
+      </c>
+      <c r="F73" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
+        <v>3.15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F74" s="6">
+        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="F71" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
-        <v>346</v>
-      </c>
-      <c r="B72" t="s">
-        <v>342</v>
-      </c>
-      <c r="C72" t="s">
-        <v>344</v>
-      </c>
-      <c r="D72">
-        <v>0.2</v>
-      </c>
-      <c r="E72">
-        <v>78.39</v>
-      </c>
-      <c r="F72" s="1">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>15.678000000000001</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="B73" t="s">
-        <v>342</v>
-      </c>
-      <c r="C73" t="s">
-        <v>343</v>
-      </c>
-      <c r="D73">
-        <v>0.2</v>
-      </c>
-      <c r="E73">
-        <v>50.47</v>
-      </c>
-      <c r="F73" s="1">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>10.094000000000001</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>304</v>
-      </c>
-      <c r="B74" t="s">
-        <v>332</v>
-      </c>
-      <c r="C74" t="s">
-        <v>310</v>
-      </c>
-      <c r="D74">
-        <v>1</v>
-      </c>
-      <c r="E74">
-        <v>5.46</v>
-      </c>
-      <c r="F74" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>5.46</v>
-      </c>
-    </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>305</v>
-      </c>
-      <c r="B75" t="s">
-        <v>332</v>
-      </c>
-      <c r="C75" t="s">
-        <v>309</v>
-      </c>
-      <c r="D75">
-        <v>1</v>
-      </c>
-      <c r="E75">
-        <v>13.9</v>
-      </c>
       <c r="F75" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>13.9</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>306</v>
-      </c>
-      <c r="B76" t="s">
-        <v>333</v>
-      </c>
-      <c r="C76" t="s">
-        <v>311</v>
-      </c>
-      <c r="D76">
-        <v>1</v>
-      </c>
-      <c r="E76">
-        <v>7.62</v>
-      </c>
-      <c r="F76" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>7.62</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>314</v>
-      </c>
-      <c r="B77" t="s">
-        <v>333</v>
-      </c>
-      <c r="C77" t="s">
-        <v>315</v>
-      </c>
-      <c r="D77">
-        <v>1</v>
-      </c>
-      <c r="E77">
-        <v>9.1300000000000008</v>
-      </c>
-      <c r="F77" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>9.1300000000000008</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>329</v>
-      </c>
-      <c r="B78" t="s">
-        <v>330</v>
-      </c>
-      <c r="C78" t="s">
-        <v>331</v>
-      </c>
-      <c r="D78">
-        <v>1</v>
-      </c>
-      <c r="E78">
-        <v>65.41</v>
-      </c>
-      <c r="F78" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>65.41</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>307</v>
-      </c>
-      <c r="B79" t="s">
-        <v>333</v>
-      </c>
-      <c r="C79" t="s">
-        <v>308</v>
-      </c>
-      <c r="D79">
-        <v>1</v>
-      </c>
-      <c r="E79">
-        <v>5.0599999999999996</v>
-      </c>
-      <c r="F79" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>5.0599999999999996</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>312</v>
-      </c>
-      <c r="B80" t="s">
-        <v>333</v>
-      </c>
-      <c r="C80" t="s">
-        <v>313</v>
-      </c>
-      <c r="D80">
-        <v>1</v>
-      </c>
-      <c r="E80">
-        <v>3.15</v>
-      </c>
-      <c r="F80" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>3.15</v>
-      </c>
-    </row>
-    <row r="81" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F81" s="6">
-        <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F82" s="6">
         <f>Table3[[#This Row],[Quantity]]*Table3[[#This Row],[Cost/Unit (USD)]]</f>
         <v>0</v>
       </c>

</xml_diff>